<commit_message>
fix board, update production files
</commit_message>
<xml_diff>
--- a/kicad-project/bom/bom.xlsx
+++ b/kicad-project/bom/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\keypad-board\kicad-project\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11055246-7FCD-434A-A831-B1BFFC12CC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71963729-D7DD-4272-9C85-9082E790F17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="975" windowWidth="32100" windowHeight="19905" xr2:uid="{D3104115-94E3-BD4B-A3F1-4563E20D6E1F}"/>
+    <workbookView xWindow="12960" yWindow="0" windowWidth="33360" windowHeight="20985" xr2:uid="{D3104115-94E3-BD4B-A3F1-4563E20D6E1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>SSD1306</t>
   </si>
   <si>
-    <t>C1, C11, C12, C13, C14, C2, C5, C9</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>SD15_SOD323</t>
   </si>
   <si>
-    <t>D17, D18</t>
-  </si>
-  <si>
     <t>D_Schottky</t>
   </si>
   <si>
@@ -275,12 +269,6 @@
     <t>4k7</t>
   </si>
   <si>
-    <t>R22, R23</t>
-  </si>
-  <si>
-    <t>56k</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -329,15 +317,9 @@
     <t>RotaryEncoder</t>
   </si>
   <si>
-    <t>SW25</t>
-  </si>
-  <si>
     <t>SW_PUSH_6mm</t>
   </si>
   <si>
-    <t>SW_RST</t>
-  </si>
-  <si>
     <t>SW26, SW27, SW28, SW32, SW33, SW34, SW38, SW39, SW40, SW44, SW45, SW46</t>
   </si>
   <si>
@@ -482,9 +464,6 @@
     <t>71-CRCW0603-4.7K-E3</t>
   </si>
   <si>
-    <t>603-RC0805FR-0756KL</t>
-  </si>
-  <si>
     <t>603-RC0805FR-1320KL</t>
   </si>
   <si>
@@ -539,19 +518,40 @@
     <t>1.78k</t>
   </si>
   <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>TDSON-8-1</t>
-  </si>
-  <si>
-    <t>BSC098N10NS5</t>
-  </si>
-  <si>
-    <t>726-BSC098N10NS5</t>
-  </si>
-  <si>
     <t>71-CRCW0805-1.78K-E3</t>
+  </si>
+  <si>
+    <t>C1, C11, C12, C13, C14, C2, C20, C21, C5, C9</t>
+  </si>
+  <si>
+    <t>D17, D18, D2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>SOIC127P600X175-8N</t>
+  </si>
+  <si>
+    <t>Si4435DDY-T1-E3</t>
+  </si>
+  <si>
+    <t>781-SI4435DDY-T1-E3</t>
+  </si>
+  <si>
+    <t>SW3, SW25</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>R22, R23, R26, R27</t>
+  </si>
+  <si>
+    <t>5.1k</t>
+  </si>
+  <si>
+    <t>603-RT0805DRE075K1L</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -739,6 +739,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1064,8 +1067,8 @@
   </sheetPr>
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1096,16 +1099,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1122,7 +1125,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F2" s="10">
         <v>1.68</v>
@@ -1134,7 +1137,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
@@ -1153,7 +1156,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F3" s="10">
         <v>5.63</v>
@@ -1165,33 +1168,33 @@
         <v>5.63</v>
       </c>
       <c r="I3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="9">
+        <v>148</v>
+      </c>
+      <c r="B4" s="23">
         <v>603</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F4" s="10">
         <v>0.43099999999999999</v>
@@ -1204,32 +1207,32 @@
       </c>
       <c r="K4" s="4" cm="1">
         <f t="array" ref="K4">SUM($C$2:$C$45*F2:F45)</f>
-        <v>256.69299999999993</v>
+        <v>255.09399999999994</v>
       </c>
       <c r="L4" s="4" cm="1">
         <f t="array" ref="L4">SUM($C$2:$C$45*G2:G45)</f>
-        <v>215.94500000000002</v>
+        <v>214.48200000000003</v>
       </c>
       <c r="M4" s="4" cm="1">
         <f t="array" ref="M4">SUM($C$2:$C$45*H2:H45)</f>
-        <v>179.36999999999998</v>
+        <v>177.10899999999998</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="9">
+        <v>11</v>
+      </c>
+      <c r="B5" s="23">
         <v>603</v>
       </c>
       <c r="C5" s="1">
         <v>6</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F5" s="10">
         <v>0.99099999999999999</v>
@@ -1243,19 +1246,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="9">
+        <v>13</v>
+      </c>
+      <c r="B6" s="23">
         <v>603</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F6" s="10">
         <v>0.82</v>
@@ -1267,26 +1270,26 @@
         <v>0.28699999999999998</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="L6" s="18"/>
       <c r="M6" s="19"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="9">
+        <v>15</v>
+      </c>
+      <c r="B7" s="23">
         <v>603</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F7" s="10">
         <v>0.64800000000000002</v>
@@ -1298,30 +1301,30 @@
         <v>0.255</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="23">
+        <v>603</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="9">
-        <v>603</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F8" s="10">
         <v>0.43099999999999999</v>
@@ -1344,7 +1347,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="9">
         <v>805</v>
@@ -1353,10 +1356,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F9" s="10">
         <v>3.06</v>
@@ -1370,19 +1373,19 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F10" s="10">
         <v>1.33</v>
@@ -1394,14 +1397,14 @@
         <v>0.69899999999999995</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="22"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="B11" s="9">
         <v>2114</v>
@@ -1410,10 +1413,10 @@
         <v>2</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F11" s="10">
         <v>2.19</v>
@@ -1425,30 +1428,30 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F12" s="10">
         <v>0.52100000000000002</v>
@@ -1460,36 +1463,36 @@
         <v>0.52100000000000002</v>
       </c>
       <c r="I12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K12" s="6">
         <f>K4+K8</f>
-        <v>265.99299999999994</v>
+        <v>264.39399999999995</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" ref="L12:M12" si="0">L4+L8</f>
-        <v>223.60500000000002</v>
+        <v>222.14200000000002</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="0"/>
-        <v>183.42999999999998</v>
+        <v>181.16899999999998</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1">
         <v>12</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F13" s="10">
         <v>0.73199999999999998</v>
@@ -1503,19 +1506,19 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F14" s="10">
         <v>5.09</v>
@@ -1529,19 +1532,19 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F15" s="10">
         <v>1.94</v>
@@ -1555,19 +1558,19 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F16" s="10">
         <v>3.44</v>
@@ -1581,19 +1584,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F17" s="10">
         <v>13.33</v>
@@ -1607,19 +1610,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F18" s="10">
         <v>5.19</v>
@@ -1633,19 +1636,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
@@ -1659,33 +1662,33 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F20" s="15">
-        <v>6.81</v>
+        <v>2.54</v>
       </c>
       <c r="G20" s="15">
-        <v>5.65</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="H20" s="15">
-        <v>4.4800000000000004</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="9">
         <v>805</v>
@@ -1694,10 +1697,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F21" s="10">
         <v>0.43099999999999999</v>
@@ -1711,19 +1714,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" s="9">
         <v>603</v>
       </c>
       <c r="C22" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F22" s="10">
         <v>0.43099999999999999</v>
@@ -1737,7 +1740,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="9">
         <v>805</v>
@@ -1746,10 +1749,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F23" s="10">
         <v>0.43099999999999999</v>
@@ -1763,7 +1766,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="9">
         <v>603</v>
@@ -1772,10 +1775,10 @@
         <v>2</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F24" s="10">
         <v>0.43099999999999999</v>
@@ -1789,7 +1792,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="9">
         <v>805</v>
@@ -1801,7 +1804,7 @@
         <v>680</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F25" s="10">
         <v>0.43099999999999999</v>
@@ -1815,19 +1818,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="9">
         <v>603</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="9">
         <v>200</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F26" s="10">
         <v>0.43099999999999999</v>
@@ -1841,7 +1844,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="9">
         <v>805</v>
@@ -1850,10 +1853,10 @@
         <v>1</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F27" s="10">
         <v>0.43099999999999999</v>
@@ -1867,7 +1870,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="9">
         <v>603</v>
@@ -1879,7 +1882,7 @@
         <v>220</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F28" s="10">
         <v>0.43099999999999999</v>
@@ -1893,7 +1896,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B29" s="9">
         <v>603</v>
@@ -1902,10 +1905,10 @@
         <v>2</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F29" s="10">
         <v>0.43099999999999999</v>
@@ -1919,45 +1922,45 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="B30" s="9">
         <v>805</v>
       </c>
       <c r="C30" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="F30" s="10">
-        <v>0.43099999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G30" s="10">
-        <v>6.9000000000000006E-2</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="H30" s="10">
-        <v>3.6999999999999998E-2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F31" s="7">
         <v>0.43099999999999999</v>
@@ -1971,7 +1974,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B32" s="9">
         <v>805</v>
@@ -1980,10 +1983,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F32" s="10">
         <v>0.43099999999999999</v>
@@ -1997,7 +2000,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B33" s="9">
         <v>805</v>
@@ -2009,7 +2012,7 @@
         <v>470</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F33" s="10">
         <v>0.43099999999999999</v>
@@ -2023,7 +2026,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B34" s="9">
         <v>603</v>
@@ -2032,10 +2035,10 @@
         <v>1</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F34" s="10">
         <v>0.43099999999999999</v>
@@ -2049,7 +2052,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B35" s="9">
         <v>603</v>
@@ -2058,10 +2061,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F35" s="10">
         <v>0.43099999999999999</v>
@@ -2075,19 +2078,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F36" s="10">
         <v>8.2899999999999991</v>
@@ -2101,19 +2104,19 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F37" s="10">
         <v>3.14</v>
@@ -2127,19 +2130,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F38" s="10">
         <v>7.96</v>
@@ -2153,19 +2156,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F39" s="10">
         <v>0.43099999999999999</v>
@@ -2179,19 +2182,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1">
         <v>12</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F40" s="10">
         <v>6.75</v>
@@ -2203,24 +2206,24 @@
         <v>5.23</v>
       </c>
       <c r="I40" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F41" s="10">
         <v>15.6</v>
@@ -2234,19 +2237,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C42" s="1">
         <v>12</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F42" s="10">
         <v>0.28000000000000003</v>
@@ -2258,24 +2261,24 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="I42" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F43" s="10">
         <v>3.14</v>
@@ -2289,19 +2292,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F44" s="10">
         <v>5.23</v>
@@ -2315,19 +2318,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F45" s="10">
         <v>17.04</v>

</xml_diff>